<commit_message>
Frontend fully functional now. Need to implement export and all done
</commit_message>
<xml_diff>
--- a/classrooms.xlsx
+++ b/classrooms.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://aucampus-my.sharepoint.com/personal/marie_doh_ashesi_edu_gh/Documents/Desktop/Documents/GitHub/cap/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\cap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{A46CBF7E-F999-4FAC-A488-CA04E0BAB5E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CE95274C-6274-4DE2-9923-30D74D2ED43D}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11AC1886-663A-43E1-BF3B-A94F422ABBE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{A0906301-E428-4BB3-8B0A-BA51242833C9}"/>
   </bookViews>
@@ -36,9 +36,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
-    <t xml:space="preserve">Classroom </t>
-  </si>
-  <si>
     <t>Capacity</t>
   </si>
   <si>
@@ -73,6 +70,9 @@
   </si>
   <si>
     <t>K</t>
+  </si>
+  <si>
+    <t>Name</t>
   </si>
 </sst>
 </file>
@@ -427,7 +427,7 @@
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -437,15 +437,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2">
         <v>20</v>
@@ -453,7 +453,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3">
         <v>20</v>
@@ -461,7 +461,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4">
         <v>20</v>
@@ -469,7 +469,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5">
         <v>35</v>
@@ -477,7 +477,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6">
         <v>35</v>
@@ -485,7 +485,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7">
         <v>35</v>
@@ -493,7 +493,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8">
         <v>35</v>
@@ -501,7 +501,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9">
         <v>35</v>
@@ -509,7 +509,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10">
         <v>35</v>
@@ -517,7 +517,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B11">
         <v>40</v>
@@ -525,7 +525,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B12">
         <v>40</v>

</xml_diff>

<commit_message>
we are in danger
</commit_message>
<xml_diff>
--- a/classrooms.xlsx
+++ b/classrooms.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://aucampus-my.sharepoint.com/personal/marie_doh_ashesi_edu_gh/Documents/Desktop/Documents/GitHub/cap/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{A46CBF7E-F999-4FAC-A488-CA04E0BAB5E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CE95274C-6274-4DE2-9923-30D74D2ED43D}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="8_{A46CBF7E-F999-4FAC-A488-CA04E0BAB5E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{46E23105-0E78-4973-9FCF-AF02AAF324BE}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{A0906301-E428-4BB3-8B0A-BA51242833C9}"/>
   </bookViews>
@@ -36,9 +36,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
-    <t xml:space="preserve">Classroom </t>
-  </si>
-  <si>
     <t>Capacity</t>
   </si>
   <si>
@@ -73,6 +70,9 @@
   </si>
   <si>
     <t>K</t>
+  </si>
+  <si>
+    <t>Name</t>
   </si>
 </sst>
 </file>
@@ -427,7 +427,7 @@
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -437,15 +437,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2">
         <v>20</v>
@@ -453,7 +453,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3">
         <v>20</v>
@@ -461,7 +461,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4">
         <v>20</v>
@@ -469,7 +469,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5">
         <v>35</v>
@@ -477,7 +477,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6">
         <v>35</v>
@@ -485,7 +485,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7">
         <v>35</v>
@@ -493,7 +493,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8">
         <v>35</v>
@@ -501,7 +501,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9">
         <v>35</v>
@@ -509,7 +509,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10">
         <v>35</v>
@@ -517,7 +517,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B11">
         <v>40</v>
@@ -525,7 +525,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B12">
         <v>40</v>

</xml_diff>